<commit_message>
Almost fully robust, just need the scraper to consistently sort the pdfs
</commit_message>
<xml_diff>
--- a/thresholds/IGCSE/biology-9-1/biology-9-1-thresholds.xlsx
+++ b/thresholds/IGCSE/biology-9-1/biology-9-1-thresholds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,11 +494,6 @@
           <t>date</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -533,17 +528,14 @@
       <c r="J2" t="n">
         <v>50</v>
       </c>
-      <c r="K2" t="n">
-        <v>35</v>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
           <t>June 2023</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
         </is>
       </c>
     </row>
@@ -580,17 +572,14 @@
       <c r="J3" t="n">
         <v>50</v>
       </c>
-      <c r="K3" t="n">
-        <v>35</v>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>June 2023</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
         </is>
       </c>
     </row>
@@ -627,158 +616,146 @@
       <c r="J4" t="n">
         <v>55</v>
       </c>
-      <c r="K4" t="n">
-        <v>37</v>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>June 2023</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>BX 21,41,51</t>
+          <t>FX 11,31,51</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>200</v>
       </c>
       <c r="C5" t="n">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>115</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="H5" t="n">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="I5" t="n">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="J5" t="n">
-        <v>52</v>
-      </c>
-      <c r="K5" t="n">
-        <v>39</v>
+        <v>73</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>June 2024</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2023</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>CX 21,41,61</t>
+          <t>GX 11,31,61</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>200</v>
       </c>
       <c r="C6" t="n">
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
+        <v>131</v>
+      </c>
+      <c r="H6" t="n">
+        <v>123</v>
+      </c>
+      <c r="I6" t="n">
         <v>98</v>
       </c>
-      <c r="H6" t="n">
-        <v>80</v>
-      </c>
-      <c r="I6" t="n">
-        <v>66</v>
-      </c>
       <c r="J6" t="n">
-        <v>52</v>
-      </c>
-      <c r="K6" t="n">
-        <v>39</v>
+        <v>73</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>June 2024</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>CY 22,42,62</t>
+          <t>GY 12,32,62</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>200</v>
       </c>
       <c r="C7" t="n">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="H7" t="n">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="I7" t="n">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="J7" t="n">
-        <v>55</v>
-      </c>
-      <c r="K7" t="n">
-        <v>37</v>
+        <v>76</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>June 2024</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2023</t>
         </is>
       </c>
     </row>
@@ -792,40 +769,37 @@
         <v>200</v>
       </c>
       <c r="C8" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D8" t="n">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E8" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F8" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G8" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H8" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I8" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J8" t="n">
-        <v>50</v>
-      </c>
-      <c r="K8" t="n">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>June 2025</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
@@ -839,40 +813,37 @@
         <v>200</v>
       </c>
       <c r="C9" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D9" t="n">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E9" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F9" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G9" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="H9" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I9" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J9" t="n">
         <v>52</v>
       </c>
-      <c r="K9" t="n">
-        <v>40</v>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>June 2025</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
@@ -886,275 +857,257 @@
         <v>200</v>
       </c>
       <c r="C10" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" t="n">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E10" t="n">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F10" t="n">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G10" t="n">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H10" t="n">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I10" t="n">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J10" t="n">
-        <v>63</v>
-      </c>
-      <c r="K10" t="n">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>June 2025</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>BY 22,42,52</t>
+          <t>FX 11,31,51</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>200</v>
       </c>
       <c r="C11" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>131</v>
       </c>
-      <c r="G11" t="n">
-        <v>116</v>
-      </c>
       <c r="H11" t="n">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="I11" t="n">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="J11" t="n">
-        <v>65</v>
-      </c>
-      <c r="K11" t="n">
-        <v>47</v>
+        <v>72</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>November 2024</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>CY 22,42,62</t>
+          <t>GX 11,31,61</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>200</v>
       </c>
       <c r="C12" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
         <v>132</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>116</v>
       </c>
-      <c r="H12" t="n">
-        <v>101</v>
-      </c>
       <c r="I12" t="n">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="J12" t="n">
-        <v>65</v>
-      </c>
-      <c r="K12" t="n">
-        <v>47</v>
+        <v>72</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>November 2024</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>BX 21,41,51</t>
+          <t>GY 12,32,62</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>200</v>
       </c>
       <c r="C13" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="H13" t="n">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I13" t="n">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="J13" t="n">
-        <v>46</v>
-      </c>
-      <c r="K13" t="n">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>June 2022</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2024</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>CX 21,41,61</t>
+          <t>BX 21,41,51</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>200</v>
       </c>
       <c r="C14" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D14" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E14" t="n">
         <v>131</v>
       </c>
       <c r="F14" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H14" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I14" t="n">
         <v>62</v>
       </c>
       <c r="J14" t="n">
-        <v>46</v>
-      </c>
-      <c r="K14" t="n">
-        <v>30</v>
+        <v>50</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>June 2022</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2025</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>CY 22,42,62</t>
+          <t>CX 21,41,61</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>200</v>
       </c>
       <c r="C15" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D15" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E15" t="n">
         <v>132</v>
       </c>
       <c r="F15" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G15" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H15" t="n">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I15" t="n">
         <v>64</v>
       </c>
       <c r="J15" t="n">
-        <v>45</v>
-      </c>
-      <c r="K15" t="n">
-        <v>26</v>
+        <v>52</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>June 2022</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>biology-9-1</t>
+          <t>June 2025</t>
         </is>
       </c>
     </row>
@@ -1168,38 +1121,655 @@
         <v>200</v>
       </c>
       <c r="C16" t="n">
+        <v>178</v>
+      </c>
+      <c r="D16" t="n">
+        <v>163</v>
+      </c>
+      <c r="E16" t="n">
+        <v>149</v>
+      </c>
+      <c r="F16" t="n">
+        <v>132</v>
+      </c>
+      <c r="G16" t="n">
+        <v>115</v>
+      </c>
+      <c r="H16" t="n">
+        <v>99</v>
+      </c>
+      <c r="I16" t="n">
+        <v>81</v>
+      </c>
+      <c r="J16" t="n">
+        <v>63</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>FX 11,31,51</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>200</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>133</v>
+      </c>
+      <c r="H17" t="n">
+        <v>117</v>
+      </c>
+      <c r="I17" t="n">
+        <v>95</v>
+      </c>
+      <c r="J17" t="n">
+        <v>74</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>GX 11,31,61</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>200</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>134</v>
+      </c>
+      <c r="H18" t="n">
+        <v>118</v>
+      </c>
+      <c r="I18" t="n">
+        <v>97</v>
+      </c>
+      <c r="J18" t="n">
+        <v>76</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>GY 12,32,62</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>200</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>127</v>
+      </c>
+      <c r="H19" t="n">
+        <v>113</v>
+      </c>
+      <c r="I19" t="n">
+        <v>95</v>
+      </c>
+      <c r="J19" t="n">
+        <v>77</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>June 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>BY 22,42,52</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>200</v>
+      </c>
+      <c r="C20" t="n">
+        <v>175</v>
+      </c>
+      <c r="D20" t="n">
         <v>161</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E20" t="n">
+        <v>147</v>
+      </c>
+      <c r="F20" t="n">
+        <v>131</v>
+      </c>
+      <c r="G20" t="n">
+        <v>116</v>
+      </c>
+      <c r="H20" t="n">
+        <v>101</v>
+      </c>
+      <c r="I20" t="n">
+        <v>83</v>
+      </c>
+      <c r="J20" t="n">
+        <v>65</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>November 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>CY 22,42,62</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>200</v>
+      </c>
+      <c r="C21" t="n">
+        <v>175</v>
+      </c>
+      <c r="D21" t="n">
+        <v>161</v>
+      </c>
+      <c r="E21" t="n">
         <v>148</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F21" t="n">
+        <v>132</v>
+      </c>
+      <c r="G21" t="n">
+        <v>116</v>
+      </c>
+      <c r="H21" t="n">
+        <v>101</v>
+      </c>
+      <c r="I21" t="n">
+        <v>83</v>
+      </c>
+      <c r="J21" t="n">
+        <v>65</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>November 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>GY 12,32,62</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>200</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>145</v>
+      </c>
+      <c r="H22" t="n">
+        <v>120</v>
+      </c>
+      <c r="I22" t="n">
+        <v>97</v>
+      </c>
+      <c r="J22" t="n">
+        <v>74</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>November 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>BX 21,41,51</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>200</v>
+      </c>
+      <c r="C23" t="n">
+        <v>160</v>
+      </c>
+      <c r="D23" t="n">
+        <v>145</v>
+      </c>
+      <c r="E23" t="n">
+        <v>130</v>
+      </c>
+      <c r="F23" t="n">
+        <v>113</v>
+      </c>
+      <c r="G23" t="n">
+        <v>96</v>
+      </c>
+      <c r="H23" t="n">
+        <v>79</v>
+      </c>
+      <c r="I23" t="n">
+        <v>62</v>
+      </c>
+      <c r="J23" t="n">
+        <v>46</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>CX 21,41,61</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>200</v>
+      </c>
+      <c r="C24" t="n">
+        <v>161</v>
+      </c>
+      <c r="D24" t="n">
+        <v>146</v>
+      </c>
+      <c r="E24" t="n">
+        <v>131</v>
+      </c>
+      <c r="F24" t="n">
+        <v>113</v>
+      </c>
+      <c r="G24" t="n">
+        <v>96</v>
+      </c>
+      <c r="H24" t="n">
+        <v>79</v>
+      </c>
+      <c r="I24" t="n">
+        <v>62</v>
+      </c>
+      <c r="J24" t="n">
+        <v>46</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>CY 22,42,62</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>200</v>
+      </c>
+      <c r="C25" t="n">
+        <v>162</v>
+      </c>
+      <c r="D25" t="n">
+        <v>147</v>
+      </c>
+      <c r="E25" t="n">
+        <v>132</v>
+      </c>
+      <c r="F25" t="n">
+        <v>115</v>
+      </c>
+      <c r="G25" t="n">
+        <v>99</v>
+      </c>
+      <c r="H25" t="n">
+        <v>83</v>
+      </c>
+      <c r="I25" t="n">
+        <v>64</v>
+      </c>
+      <c r="J25" t="n">
+        <v>45</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>FX 11,31,51</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>200</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>127</v>
+      </c>
+      <c r="H26" t="n">
+        <v>108</v>
+      </c>
+      <c r="I26" t="n">
+        <v>90</v>
+      </c>
+      <c r="J26" t="n">
+        <v>72</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>GX 11,31,61</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>200</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>127</v>
+      </c>
+      <c r="H27" t="n">
+        <v>108</v>
+      </c>
+      <c r="I27" t="n">
+        <v>90</v>
+      </c>
+      <c r="J27" t="n">
+        <v>72</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>GY 12,32,62</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>200</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>125</v>
+      </c>
+      <c r="H28" t="n">
+        <v>110</v>
+      </c>
+      <c r="I28" t="n">
+        <v>88</v>
+      </c>
+      <c r="J28" t="n">
+        <v>67</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>June 2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>CY 22,42,62</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>200</v>
+      </c>
+      <c r="C29" t="n">
+        <v>161</v>
+      </c>
+      <c r="D29" t="n">
+        <v>148</v>
+      </c>
+      <c r="E29" t="n">
         <v>135</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F29" t="n">
         <v>121</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G29" t="n">
         <v>107</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H29" t="n">
         <v>94</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I29" t="n">
         <v>75</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J29" t="n">
         <v>56</v>
       </c>
-      <c r="K16" t="n">
-        <v>38</v>
-      </c>
-      <c r="L16" t="inlineStr">
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
         <is>
           <t>November 2022</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>GY 12,32,62</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>200</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>140</v>
+      </c>
+      <c r="H30" t="n">
+        <v>113</v>
+      </c>
+      <c r="I30" t="n">
+        <v>93</v>
+      </c>
+      <c r="J30" t="n">
+        <v>73</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>November 2022</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>